<commit_message>
Uploaded updated data dictionary
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29609"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4F90BC2-D3DC-4C7B-BBDA-BDAC98FCFC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0380F093-8CB7-4B2A-8D91-142D62F1D1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>Variable</t>
   </si>
@@ -45,7 +45,10 @@
     <t>id</t>
   </si>
   <si>
-    <t>Patient identifier from FMP "</t>
+    <t xml:space="preserve">Patient identifier from FMP </t>
+  </si>
+  <si>
+    <t>Unique ID</t>
   </si>
   <si>
     <t>gender</t>
@@ -54,24 +57,36 @@
     <t>Patient gender</t>
   </si>
   <si>
+    <t>Female, Male, or Other</t>
+  </si>
+  <si>
     <t>race</t>
   </si>
   <si>
     <t>Patient race</t>
   </si>
   <si>
+    <t>American Indian and Alaska Native, Asian, Black or African American, More Than One Race, Native Hawaiian and Other Pacific Islander,  Other, Patient Refused, Unknown, White or Caucasian</t>
+  </si>
+  <si>
     <t>nes_es</t>
   </si>
   <si>
     <t>Does patient have comorbid epilepsy and functional seizures</t>
   </si>
   <si>
+    <t>1= yes, 0 = no</t>
+  </si>
+  <si>
     <t>veteran</t>
   </si>
   <si>
     <t xml:space="preserve">Is patient a veteran </t>
   </si>
   <si>
+    <t>1=yes, 0 = no</t>
+  </si>
+  <si>
     <t>substance_use</t>
   </si>
   <si>
@@ -84,39 +99,51 @@
     <t>How many failed anti-seizure medications per patient</t>
   </si>
   <si>
+    <t>Count</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
     <t>Patient Age</t>
   </si>
   <si>
+    <t>Numeric (years)</t>
+  </si>
+  <si>
     <t>trauma_hx</t>
   </si>
   <si>
     <t>Does patient have history of trauma</t>
   </si>
   <si>
-    <t>1= yes, 0 = no</t>
-  </si>
-  <si>
     <t>suicidality</t>
   </si>
   <si>
     <t>Does patient have suicidal thoughts and/or history of suicide attempt(s)</t>
   </si>
   <si>
+    <t>No, Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">insurance </t>
   </si>
   <si>
     <t>What health insurance group does patient have</t>
   </si>
   <si>
+    <t>Medicaid/CHF, Medicare, Other, Private, Veteran/ASM</t>
+  </si>
+  <si>
     <t>employment</t>
   </si>
   <si>
     <t>Is patient employed</t>
   </si>
   <si>
+    <t>Employed = Employed or Active Duty, Unemployed= Unemployed, Not in labor force= Student, Retired.</t>
+  </si>
+  <si>
     <t>driving</t>
   </si>
   <si>
@@ -129,12 +156,18 @@
     <t>What is patient's marital status</t>
   </si>
   <si>
+    <t>Has_Partner, Single</t>
+  </si>
+  <si>
     <t>education</t>
   </si>
   <si>
     <t>Highest level of education</t>
   </si>
   <si>
+    <t>&lt; High School, High School Diploma, Some College, Partial College or 2 Year Degree, 4 Year College Degree, Graduate or Professional Degree, Unknown</t>
+  </si>
+  <si>
     <t>psych_care_entered</t>
   </si>
   <si>
@@ -147,12 +180,18 @@
     <t>How long between symptom onset and diagnosis</t>
   </si>
   <si>
+    <t>Numeric (months)</t>
+  </si>
+  <si>
     <t>n_visits_scheduled</t>
   </si>
   <si>
     <t>Number of total visits  scheduled</t>
   </si>
   <si>
+    <t>Numeric</t>
+  </si>
+  <si>
     <t>n_visits_completed</t>
   </si>
   <si>
@@ -171,6 +210,9 @@
     <t>BIPQ Affect Life Subscale Score</t>
   </si>
   <si>
+    <t>Numeric, 0-10 possible values</t>
+  </si>
+  <si>
     <t>how_long</t>
   </si>
   <si>
@@ -219,6 +261,9 @@
     <t>BIPQ Total Score (0-80)</t>
   </si>
   <si>
+    <t>Numeric, 0-80 possible values</t>
+  </si>
+  <si>
     <t>total_conditions</t>
   </si>
   <si>
@@ -249,24 +294,36 @@
     <t>Race restricted to white/other</t>
   </si>
   <si>
+    <t>Other, White</t>
+  </si>
+  <si>
     <t>disability</t>
   </si>
   <si>
     <t>Is patient on disability-  Yes if completely, long term, partially, SSDI, SSI, Short Term, Spouse/parent disability, retired. No if "No" , Not pursuing</t>
   </si>
   <si>
+    <t>Disability, No Disability</t>
+  </si>
+  <si>
     <t>freqbaseline_monthly</t>
   </si>
   <si>
     <t>Number of seizures monthly</t>
   </si>
   <si>
+    <t>Numeric (monthly)</t>
+  </si>
+  <si>
     <t>visit_prop</t>
   </si>
   <si>
     <t>Proportion of completed visits to scheduled</t>
   </si>
   <si>
+    <t>Proportion, 0-1</t>
+  </si>
+  <si>
     <t>visit_complete_50</t>
   </si>
   <si>
@@ -280,6 +337,15 @@
   </si>
   <si>
     <t>Low= score &lt; median total score , High = score &gt; median total score</t>
+  </si>
+  <si>
+    <t>education3</t>
+  </si>
+  <si>
+    <t>Time spent in education- Classification derived from Loucks, E.B., Abrahamowicz, M., Xiao, Y. et al. Associations of education with 30 year life course blood pressure trajectories: Framingham Offspring Study. BMC Public Health 11, 139 (2011). https://doi.org/10.1186/1471-2458-11-139</t>
+  </si>
+  <si>
+    <t>≤12 years (reflecting high school or less), 13-16 years (some post-secondary education, including technical school and college degree), ≥17 years education (more than an undergraduate college degree)</t>
   </si>
 </sst>
 </file>
@@ -674,17 +740,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -706,318 +772,437 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="159">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.75">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="87">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="130.5">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>56</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29.25">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29.25">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="29.25">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29.25">
       <c r="A25" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>65</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29.25">
       <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29.25">
+      <c r="A27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29.25">
+      <c r="A28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29.25">
+      <c r="A29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29.25">
+      <c r="A30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="43.5">
       <c r="A36" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29.25">
       <c r="A37" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>95</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29.25">
       <c r="A39" s="2" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="57.75">
       <c r="A40" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>82</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="159">
+      <c r="A41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1026,8 +1211,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E078C362419F04EB99D388536984176" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="158d4a53e617032ea5de8b2c26100f9b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b255dc67-9167-4049-a4bf-c673fab073d8" xmlns:ns3="b6a82f82-b2b5-443d-9ae4-df21184f170b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce6f8f0a719a106f4e486ba2f71a50c1" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b6a82f82-b2b5-443d-9ae4-df21184f170b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b255dc67-9167-4049-a4bf-c673fab073d8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E078C362419F04EB99D388536984176" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0edfaceebdbff7527aca8aca48f1d813">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b255dc67-9167-4049-a4bf-c673fab073d8" xmlns:ns3="b6a82f82-b2b5-443d-9ae4-df21184f170b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68665fba23bd277fd5ffe283298e8881" ns2:_="" ns3:_="">
     <xsd:import namespace="b255dc67-9167-4049-a4bf-c673fab073d8"/>
     <xsd:import namespace="b6a82f82-b2b5-443d-9ae4-df21184f170b"/>
     <xsd:element name="properties">
@@ -1268,17 +1464,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b6a82f82-b2b5-443d-9ae4-df21184f170b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b255dc67-9167-4049-a4bf-c673fab073d8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1289,11 +1474,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C488CED3-6AC0-41CE-AE40-A66D88EA3F39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5E82CA-0CD5-455F-B97A-DE7095ECDA02}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5E82CA-0CD5-455F-B97A-DE7095ECDA02}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53EDC40D-3BC7-4671-AA58-F6211681FF26}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>